<commit_message>
chore(ProjectLab): update index and notes
</commit_message>
<xml_diff>
--- a/projects/2025-11-26_证券市赚率/市赚率统计.xlsx
+++ b/projects/2025-11-26_证券市赚率/市赚率统计.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quant\ProjectLab\projects\2025-11-26_证券市赚率\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3697AE6-A4C5-4DA7-B86E-A89ECA0760B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B03D0A8-3E55-4776-9A85-6546F11235A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="贵州茅台" sheetId="1" r:id="rId1"/>
     <sheet name="山西汾酒" sheetId="5" r:id="rId2"/>
-    <sheet name="对比" sheetId="8" r:id="rId3"/>
-    <sheet name="备注" sheetId="6" r:id="rId4"/>
+    <sheet name="美的集团" sheetId="10" r:id="rId3"/>
+    <sheet name="对比" sheetId="8" r:id="rId4"/>
+    <sheet name="备注" sheetId="6" r:id="rId5"/>
+    <sheet name="数据处理" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
   <si>
     <t>年份</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,7 +152,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="182" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
+    <numFmt numFmtId="177" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -452,19 +454,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="182" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2002,7 +2004,7 @@
         <v>87.83</v>
       </c>
       <c r="E2" s="11">
-        <f>D2/(B2*C2)</f>
+        <f t="shared" ref="E2:E20" si="0">D2/(B2*C2)</f>
         <v>2.1239036493031964</v>
       </c>
     </row>
@@ -2020,7 +2022,7 @@
         <v>230</v>
       </c>
       <c r="E3" s="5">
-        <f>D3/(B3*C3)</f>
+        <f t="shared" si="0"/>
         <v>1.9493177387914231</v>
       </c>
     </row>
@@ -2038,7 +2040,7 @@
         <v>108.7</v>
       </c>
       <c r="E4" s="5">
-        <f>D4/(B4*C4)</f>
+        <f t="shared" si="0"/>
         <v>0.69089919863320182</v>
       </c>
     </row>
@@ -2056,7 +2058,7 @@
         <v>169.82</v>
       </c>
       <c r="E5" s="5">
-        <f>D5/(B5*C5)</f>
+        <f t="shared" si="0"/>
         <v>1.2211424030949223</v>
       </c>
     </row>
@@ -2074,7 +2076,7 @@
         <v>183.92</v>
       </c>
       <c r="E6" s="5">
-        <f>D6/(B6*C6)</f>
+        <f t="shared" si="0"/>
         <v>1.2243164477249096</v>
       </c>
     </row>
@@ -2092,7 +2094,7 @@
         <v>193.3</v>
       </c>
       <c r="E7" s="5">
-        <f>D7/(B7*C7)</f>
+        <f t="shared" si="0"/>
         <v>0.5669020693538549</v>
       </c>
     </row>
@@ -2110,7 +2112,7 @@
         <v>209.02</v>
       </c>
       <c r="E8" s="5">
-        <f>D8/(B8*C8)</f>
+        <f t="shared" si="0"/>
         <v>0.39285279316042948</v>
       </c>
     </row>
@@ -2128,7 +2130,7 @@
         <v>128.38</v>
       </c>
       <c r="E9" s="5">
-        <f>D9/(B9*C9)</f>
+        <f t="shared" si="0"/>
         <v>0.25931424531636615</v>
       </c>
       <c r="H9" s="1"/>
@@ -2147,7 +2149,7 @@
         <v>186.62</v>
       </c>
       <c r="E10" s="5">
-        <f>D10/(B10*C10)</f>
+        <f t="shared" si="0"/>
         <v>0.46716291774808555</v>
       </c>
     </row>
@@ -2165,7 +2167,7 @@
         <v>218.19</v>
       </c>
       <c r="E11" s="5">
-        <f>D11/(B11*C11)</f>
+        <f t="shared" si="0"/>
         <v>0.66440195298059745</v>
       </c>
     </row>
@@ -2183,7 +2185,7 @@
         <v>334.15</v>
       </c>
       <c r="E12" s="5">
-        <f>D12/(B12*C12)</f>
+        <f t="shared" si="0"/>
         <v>0.998864077960123</v>
       </c>
     </row>
@@ -2201,7 +2203,7 @@
         <v>697.49</v>
       </c>
       <c r="E13" s="5">
-        <f>D13/(B13*C13)</f>
+        <f t="shared" si="0"/>
         <v>0.97153318212949458</v>
       </c>
     </row>
@@ -2219,7 +2221,7 @@
         <v>590.01</v>
       </c>
       <c r="E14" s="5">
-        <f>D14/(B14*C14)</f>
+        <f t="shared" si="0"/>
         <v>0.59777073793648172</v>
       </c>
     </row>
@@ -2237,7 +2239,7 @@
         <v>1183</v>
       </c>
       <c r="E15" s="5">
-        <f>D15/(B15*C15)</f>
+        <f t="shared" si="0"/>
         <v>1.079458354624425</v>
       </c>
     </row>
@@ -2255,7 +2257,7 @@
         <v>1998</v>
       </c>
       <c r="E16" s="5">
-        <f>D16/(B16*C16)</f>
+        <f t="shared" si="0"/>
         <v>1.6876269996331652</v>
       </c>
     </row>
@@ -2273,7 +2275,7 @@
         <v>2050</v>
       </c>
       <c r="E17" s="5">
-        <f>D17/(B17*C17)</f>
+        <f t="shared" si="0"/>
         <v>1.6359324176367878</v>
       </c>
     </row>
@@ -2291,7 +2293,7 @@
         <v>1727</v>
       </c>
       <c r="E18" s="5">
-        <f>D18/(B18*C18)</f>
+        <f t="shared" si="0"/>
         <v>1.1405384411316069</v>
       </c>
     </row>
@@ -2309,7 +2311,7 @@
         <v>1726</v>
       </c>
       <c r="E19" s="5">
-        <f>D19/(B19*C19)</f>
+        <f t="shared" si="0"/>
         <v>0.84805639820719103</v>
       </c>
     </row>
@@ -2327,7 +2329,7 @@
         <v>1524</v>
       </c>
       <c r="E20" s="8">
-        <f>D20/(B20*C20)</f>
+        <f t="shared" si="0"/>
         <v>0.61614107690059194</v>
       </c>
     </row>
@@ -2389,7 +2391,7 @@
         <v>30.99</v>
       </c>
       <c r="E2" s="11">
-        <f>D2/(B2*C2)</f>
+        <f t="shared" ref="E2:E20" si="0">D2/(B2*C2)</f>
         <v>2.2349632193855475</v>
       </c>
     </row>
@@ -2407,7 +2409,7 @@
         <v>36.799999999999997</v>
       </c>
       <c r="E3" s="5">
-        <f>D3/(B3*C3)</f>
+        <f t="shared" si="0"/>
         <v>1.6498690864746601</v>
       </c>
     </row>
@@ -2425,7 +2427,7 @@
         <v>10.85</v>
       </c>
       <c r="E4" s="5">
-        <f>D4/(B4*C4)</f>
+        <f t="shared" si="0"/>
         <v>0.87962084693300135</v>
       </c>
     </row>
@@ -2443,7 +2445,7 @@
         <v>42.93</v>
       </c>
       <c r="E5" s="5">
-        <f>D5/(B5*C5)</f>
+        <f t="shared" si="0"/>
         <v>2.2487624734815745</v>
       </c>
     </row>
@@ -2461,7 +2463,7 @@
         <v>68.53</v>
       </c>
       <c r="E6" s="5">
-        <f>D6/(B6*C6)</f>
+        <f t="shared" si="0"/>
         <v>4.1685401678657072</v>
       </c>
     </row>
@@ -2479,7 +2481,7 @@
         <v>63.14</v>
       </c>
       <c r="E7" s="5">
-        <f>D7/(B7*C7)</f>
+        <f t="shared" si="0"/>
         <v>1.9744382482398606</v>
       </c>
     </row>
@@ -2497,7 +2499,7 @@
         <v>41.66</v>
       </c>
       <c r="E8" s="5">
-        <f>D8/(B8*C8)</f>
+        <f t="shared" si="0"/>
         <v>0.60950716473770183</v>
       </c>
     </row>
@@ -2515,7 +2517,7 @@
         <v>19.3</v>
       </c>
       <c r="E9" s="5">
-        <f>D9/(B9*C9)</f>
+        <f t="shared" si="0"/>
         <v>0.66926714519383146</v>
       </c>
       <c r="H9" s="1"/>
@@ -2534,7 +2536,7 @@
         <v>22.89</v>
       </c>
       <c r="E10" s="5">
-        <f>D10/(B10*C10)</f>
+        <f t="shared" si="0"/>
         <v>5.7177828291659374</v>
       </c>
     </row>
@@ -2552,7 +2554,7 @@
         <v>19.27</v>
       </c>
       <c r="E11" s="5">
-        <f>D11/(B11*C11)</f>
+        <f t="shared" si="0"/>
         <v>2.5755971856889288</v>
       </c>
     </row>
@@ -2570,7 +2572,7 @@
         <v>25.02</v>
       </c>
       <c r="E12" s="5">
-        <f>D12/(B12*C12)</f>
+        <f t="shared" si="0"/>
         <v>2.8004357128754229</v>
       </c>
     </row>
@@ -2588,7 +2590,7 @@
         <v>56.99</v>
       </c>
       <c r="E13" s="5">
-        <f>D13/(B13*C13)</f>
+        <f t="shared" si="0"/>
         <v>2.7521995623331432</v>
       </c>
     </row>
@@ -2606,7 +2608,7 @@
         <v>35.049999999999997</v>
       </c>
       <c r="E14" s="5">
-        <f>D14/(B14*C14)</f>
+        <f t="shared" si="0"/>
         <v>0.810411013876433</v>
       </c>
     </row>
@@ -2624,7 +2626,7 @@
         <v>89.7</v>
       </c>
       <c r="E15" s="5">
-        <f>D15/(B15*C15)</f>
+        <f t="shared" si="0"/>
         <v>2.0144096991334264</v>
       </c>
     </row>
@@ -2642,7 +2644,7 @@
         <v>375.29</v>
       </c>
       <c r="E16" s="5">
-        <f>D16/(B16*C16)</f>
+        <f t="shared" si="0"/>
         <v>4.0931304142308189</v>
       </c>
     </row>
@@ -2660,7 +2662,7 @@
         <v>315.77999999999997</v>
       </c>
       <c r="E17" s="5">
-        <f>D17/(B17*C17)</f>
+        <f t="shared" si="0"/>
         <v>1.7525844293313035</v>
       </c>
     </row>
@@ -2678,7 +2680,7 @@
         <v>284.99</v>
       </c>
       <c r="E18" s="5">
-        <f>D18/(B18*C18)</f>
+        <f t="shared" si="0"/>
         <v>0.95986498637920636</v>
       </c>
     </row>
@@ -2696,7 +2698,7 @@
         <v>230.72</v>
       </c>
       <c r="E19" s="5">
-        <f>D19/(B19*C19)</f>
+        <f t="shared" si="0"/>
         <v>0.62506477000688687</v>
       </c>
     </row>
@@ -2714,7 +2716,7 @@
         <v>184.21</v>
       </c>
       <c r="E20" s="8">
-        <f>D20/(B20*C20)</f>
+        <f t="shared" si="0"/>
         <v>0.4623787770847167</v>
       </c>
     </row>
@@ -2728,6 +2730,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEF6A54-A8C7-4A67-BD0E-F812F01B6120}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="25.75" style="20" customWidth="1"/>
+    <col min="3" max="3" width="24.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="17">
+        <v>3.18</v>
+      </c>
+      <c r="C2" s="10">
+        <v>18.25</v>
+      </c>
+      <c r="D2" s="10">
+        <v>50</v>
+      </c>
+      <c r="E2" s="11">
+        <f t="shared" ref="E2:E13" si="0">D2/(B2*C2)</f>
+        <v>0.86154906521926422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18">
+        <v>2.25</v>
+      </c>
+      <c r="C3" s="4">
+        <v>26.61</v>
+      </c>
+      <c r="D3" s="4">
+        <v>27.44</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45830723621028019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="18">
+        <v>1.71</v>
+      </c>
+      <c r="C4" s="4">
+        <v>24.96</v>
+      </c>
+      <c r="D4" s="4">
+        <v>32.82</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76894961763382808</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2.1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>24.7</v>
+      </c>
+      <c r="D5" s="4">
+        <v>28.17</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54308849045691154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2.41</v>
+      </c>
+      <c r="C6" s="4">
+        <v>23.38</v>
+      </c>
+      <c r="D6" s="4">
+        <v>55.43</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.98374679213002558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="18">
+        <v>3.05</v>
+      </c>
+      <c r="C7" s="4">
+        <v>25.44</v>
+      </c>
+      <c r="D7" s="4">
+        <v>36.86</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.47504897412104341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18">
+        <v>3.38</v>
+      </c>
+      <c r="C8" s="4">
+        <v>24.8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>58.25</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69490837946172934</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="18">
+        <v>3.55</v>
+      </c>
+      <c r="C9" s="4">
+        <v>22.56</v>
+      </c>
+      <c r="D9" s="4">
+        <v>98.44</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2291479372690042</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="18">
+        <v>3.78</v>
+      </c>
+      <c r="C10" s="4">
+        <v>21.86</v>
+      </c>
+      <c r="D10" s="4">
+        <v>73.81</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.89325045866674424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="18">
+        <v>4.2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>51.8</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5736434108527132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="18">
+        <v>4.82</v>
+      </c>
+      <c r="C12" s="4">
+        <v>21.74</v>
+      </c>
+      <c r="D12" s="4">
+        <v>54.63</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.52134429145655758</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18">
+        <v>5.04</v>
+      </c>
+      <c r="C13" s="4">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="D13" s="4">
+        <v>75.22</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75605892475193393</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
+    <sortCondition ref="A1:A13"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67492A48-1518-4596-A634-DDDF2A28A77A}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -3009,7 +3272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5A34B9-F5D8-48CF-9526-1C05F76AAEC3}">
   <dimension ref="B3:B5"/>
   <sheetViews>
@@ -3041,4 +3304,120 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578A2E56-3B94-4C25-B575-178DF8D9B85B}">
+  <dimension ref="A2:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="B2">
+        <v>21.74</v>
+      </c>
+      <c r="C2">
+        <v>21.5</v>
+      </c>
+      <c r="D2">
+        <v>21.86</v>
+      </c>
+      <c r="E2">
+        <v>22.56</v>
+      </c>
+      <c r="F2">
+        <v>24.8</v>
+      </c>
+      <c r="G2">
+        <v>25.44</v>
+      </c>
+      <c r="H2">
+        <v>23.38</v>
+      </c>
+      <c r="I2">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>19.739999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>21.74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>21.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>22.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>25.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>23.38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14">
+        <v>1.71</v>
+      </c>
+      <c r="C14">
+        <v>2.25</v>
+      </c>
+      <c r="D14">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18">
+        <v>3.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>